<commit_message>
Fixed two colors in the layout.
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="480" yWindow="48" windowWidth="22992" windowHeight="10032"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -163,7 +163,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +194,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -207,12 +213,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,19 +524,19 @@
   <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB16" sqref="AB16"/>
+      <selection activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="7" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="17" width="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.44140625" bestFit="1" customWidth="1"/>
     <col min="19" max="24" width="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -708,7 +715,7 @@
       <c r="H3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -1247,7 +1254,7 @@
       <c r="H10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="5" t="s">
         <v>24</v>
       </c>
       <c r="J10" s="1" t="s">
@@ -2002,7 +2009,7 @@
       <c r="J20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="K20" s="5" t="s">
         <v>13</v>
       </c>
       <c r="L20" s="3" t="s">
@@ -2276,7 +2283,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2288,7 +2295,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed indentation and Sysout messages.
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\School\Software Engineering\Clue\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="480" yWindow="48" windowWidth="22992" windowHeight="10032"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,9 +126,6 @@
     <t>OL</t>
   </si>
   <si>
-    <t>OR</t>
-  </si>
-  <si>
     <t>O = Lounge</t>
   </si>
   <si>
@@ -147,6 +139,9 @@
   </si>
   <si>
     <t>BL</t>
+  </si>
+  <si>
+    <t>OD</t>
   </si>
 </sst>
 </file>
@@ -285,7 +280,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -320,7 +315,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -532,22 +527,22 @@
   <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="7" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="17" width="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.44140625" bestFit="1" customWidth="1"/>
     <col min="19" max="24" width="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -621,7 +616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -698,7 +693,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -775,7 +770,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -852,7 +847,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -929,7 +924,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1006,7 +1001,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1083,9 +1078,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>5</v>
@@ -1151,7 +1146,7 @@
         <v>34</v>
       </c>
       <c r="W8" s="4" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="X8">
         <v>7</v>
@@ -1160,7 +1155,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -1234,10 +1229,10 @@
         <v>8</v>
       </c>
       <c r="Z9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1311,10 +1306,10 @@
         <v>9</v>
       </c>
       <c r="Z10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -1388,12 +1383,12 @@
         <v>10</v>
       </c>
       <c r="Z11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>5</v>
@@ -1465,10 +1460,10 @@
         <v>11</v>
       </c>
       <c r="Z12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -1542,7 +1537,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -1616,7 +1611,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1690,7 +1685,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1764,7 +1759,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
@@ -1838,7 +1833,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
@@ -1912,7 +1907,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -1986,7 +1981,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>8</v>
       </c>
@@ -2018,7 +2013,7 @@
         <v>3</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>7</v>
@@ -2060,7 +2055,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>8</v>
       </c>
@@ -2134,7 +2129,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>8</v>
       </c>
@@ -2208,7 +2203,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0</v>
       </c>
@@ -2291,7 +2286,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2303,7 +2298,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>